<commit_message>
Results Characterization last commit
</commit_message>
<xml_diff>
--- a/src/modelsTeste.xlsx
+++ b/src/modelsTeste.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,11 +825,11 @@
         <v>1</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Multi-Model</t>
         </is>
       </c>
     </row>
@@ -3702,11 +3702,11 @@
         <v>1</v>
       </c>
       <c r="D156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Multi-Model</t>
         </is>
       </c>
     </row>
@@ -5119,11 +5119,11 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>vert.x</t>
+          <t>validator</t>
         </is>
       </c>
       <c r="C224" t="b">
@@ -5140,11 +5140,11 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>vespa</t>
+          <t>vert.x</t>
         </is>
       </c>
       <c r="C225" t="b">
@@ -5161,32 +5161,32 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>visualvm</t>
+          <t>vespa</t>
         </is>
       </c>
       <c r="C226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D226" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>NoSQL</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>wildfly</t>
+          <t>visualvm</t>
         </is>
       </c>
       <c r="C227" t="b">
@@ -5203,32 +5203,32 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>xxl-job</t>
+          <t>wildfly</t>
         </is>
       </c>
       <c r="C228" t="b">
         <v>1</v>
       </c>
       <c r="D228" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Multi-Model</t>
+          <t>Relational</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>yacy_search_server</t>
+          <t>xxl-job</t>
         </is>
       </c>
       <c r="C229" t="b">
@@ -5245,53 +5245,53 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>zaproxy</t>
+          <t>yacy_search_server</t>
         </is>
       </c>
       <c r="C230" t="b">
         <v>1</v>
       </c>
       <c r="D230" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Multi-Model</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>zeppelin</t>
+          <t>zaproxy</t>
         </is>
       </c>
       <c r="C231" t="b">
         <v>1</v>
       </c>
       <c r="D231" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Multi-Model</t>
+          <t>Relational</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>zipkin</t>
+          <t>zeppelin</t>
         </is>
       </c>
       <c r="C232" t="b">
@@ -5308,20 +5308,41 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>zipkin</t>
+        </is>
+      </c>
+      <c r="C233" t="b">
+        <v>1</v>
+      </c>
+      <c r="D233" t="b">
+        <v>1</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Multi-Model</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
         <v>358</v>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B234" t="inlineStr">
         <is>
           <t>zookeeper</t>
         </is>
       </c>
-      <c r="C233" t="b">
-        <v>1</v>
-      </c>
-      <c r="D233" t="b">
-        <v>0</v>
-      </c>
-      <c r="E233" t="inlineStr">
+      <c r="C234" t="b">
+        <v>1</v>
+      </c>
+      <c r="D234" t="b">
+        <v>0</v>
+      </c>
+      <c r="E234" t="inlineStr">
         <is>
           <t>Relational</t>
         </is>

</xml_diff>